<commit_message>
APITesting generated file - 2023-11-24 11:51
</commit_message>
<xml_diff>
--- a/ExcelTest.xlsx
+++ b/ExcelTest.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -849,7 +849,7 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>data.id: contains 7</t>
         </is>
       </c>
     </row>
@@ -866,12 +866,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>/users/3</t>
+          <t>/register</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>GET</t>
+          <t>POST</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -891,7 +891,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>id=3</t>
+          <t>None</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -901,17 +901,17 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>BasicAuth</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>username: eve.holt@reqres.in, password: cityslicka</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>400</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -921,7 +921,7 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>data.last_name: 'Wong'</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -938,12 +938,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>/register</t>
+          <t>/users/3</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>POST</t>
+          <t>GET</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -963,7 +963,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>id=3</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -973,17 +973,17 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>BasicAuth</t>
+          <t>None</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>username:password</t>
+          <t>None</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>400</t>
+          <t>200</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -993,79 +993,7 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Rest Assured</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>https://reqres.in/api</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>/users/2</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>GET</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>200</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>Cache-Control: 'max-age=14400'</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>None</t>
+          <t>data.last_name: 'Wong'</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
APITesting generated file - 2023-11-24 11:54
</commit_message>
<xml_diff>
--- a/ExcelTest.xlsx
+++ b/ExcelTest.xlsx
@@ -849,7 +849,7 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>data.id: contains 7</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -906,7 +906,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>username: eve.holt@reqres.in, password: cityslicka</t>
+          <t>username and password</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -938,7 +938,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>/users/3</t>
+          <t>/users/{id}</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">

</xml_diff>

<commit_message>
APITesting generated file - 2023-11-24 12:03
</commit_message>
<xml_diff>
--- a/ExcelTest.xlsx
+++ b/ExcelTest.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -660,7 +660,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>ContentType.JSON</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -849,7 +849,7 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>data array should not be null, should have more than 1 item</t>
         </is>
       </c>
     </row>
@@ -866,12 +866,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>/users/{id}</t>
+          <t>/register</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>GET</t>
+          <t>POST</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -891,7 +891,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>id=3</t>
+          <t>None</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -901,17 +901,17 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>BasicAuth</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>{username: 'testuser', password: 'testpass'}</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>400</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -921,7 +921,7 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>data.last_name: 'Wong'</t>
+          <t>response should contain error message</t>
         </is>
       </c>
     </row>
@@ -938,12 +938,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>/register</t>
+          <t>/users/5</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>POST</t>
+          <t>GET</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -963,7 +963,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>id=5</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -973,17 +973,17 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>BasicAuth</t>
+          <t>None</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>username:password</t>
+          <t>None</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>400</t>
+          <t>404</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -994,6 +994,78 @@
       <c r="N8" t="inlineStr">
         <is>
           <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Rest Assured</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>https://reqres.in/api</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>/users?page=3</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>data array should not be null, should have more than 1 item. Page number should be 3.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
APITesting generated file - 2023-11-27 01:12
</commit_message>
<xml_diff>
--- a/ExcelTest.xlsx
+++ b/ExcelTest.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -660,7 +660,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>ContentType.JSON</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -824,7 +824,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>{"page": 2}</t>
+          <t>page=2</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -849,7 +849,7 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>data: contains only one page with 6 users</t>
         </is>
       </c>
     </row>
@@ -866,12 +866,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>/users/3</t>
+          <t>/register</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>GET</t>
+          <t>POST</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -891,7 +891,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>{"id": 3}</t>
+          <t>None</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -901,17 +901,17 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>BasicAuth</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>username: 'testuser', password: 'testpass'</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>400</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -921,7 +921,7 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>data.last_name: 'Wong'</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -938,12 +938,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>/register</t>
+          <t>/users/3</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>POST</t>
+          <t>GET</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -963,7 +963,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>id=3</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -973,17 +973,17 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>BasicAuth</t>
+          <t>None</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>username and password</t>
+          <t>None</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>400</t>
+          <t>200</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -993,79 +993,7 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Rest Assured</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>https://reqres.in/api</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>/users</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>POST</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>ContentType.JSON</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>{"name": "", "job": ""}</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>400</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>None</t>
+          <t>data.last_name: 'Wong'</t>
         </is>
       </c>
     </row>

</xml_diff>